<commit_message>
#5 Write a "CREATE DATABASE" script
I wroti the script for the database, maybe I will add some constrains
later.
</commit_message>
<xml_diff>
--- a/TimeRecorder_Desktop/Planing/TimeRecorderDatabasePlaning.xlsx
+++ b/TimeRecorder_Desktop/Planing/TimeRecorderDatabasePlaning.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ERM" sheetId="1" r:id="rId1"/>
@@ -124,9 +124,6 @@
     <t>VARCHAR(50)</t>
   </si>
   <si>
-    <t>VARCHAR(8)</t>
-  </si>
-  <si>
     <t>NVARCHAR(MAX)</t>
   </si>
   <si>
@@ -236,6 +233,9 @@
   </si>
   <si>
     <t>Development</t>
+  </si>
+  <si>
+    <t>VARCHAR(100)</t>
   </si>
 </sst>
 </file>
@@ -626,18 +626,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -667,12 +655,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -682,15 +664,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
@@ -721,6 +694,33 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -4528,8 +4528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:L15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4546,243 +4546,243 @@
   <sheetData>
     <row r="1" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="26"/>
-      <c r="F2" s="10" t="s">
+      <c r="C2" s="37"/>
+      <c r="D2" s="20"/>
+      <c r="F2" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="11"/>
-      <c r="H2" s="26"/>
-      <c r="J2" s="8" t="s">
+      <c r="G2" s="39"/>
+      <c r="H2" s="20"/>
+      <c r="J2" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="9"/>
+      <c r="K2" s="37"/>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="F3" s="12" t="s">
+      <c r="D3" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="17" t="s">
+      <c r="G3" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="H3" s="18" t="s">
-        <v>41</v>
+      <c r="H3" s="14" t="s">
+        <v>40</v>
       </c>
       <c r="J3" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="14" t="s">
+      <c r="K3" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="L3" s="19" t="s">
-        <v>41</v>
+      <c r="L3" s="15" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="F4" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="G4" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="G4" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="H4" s="18" t="s">
-        <v>41</v>
+      <c r="H4" s="14" t="s">
+        <v>40</v>
       </c>
       <c r="J4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="K4" s="16" t="s">
+      <c r="K4" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="L4" s="19" t="s">
-        <v>41</v>
+      <c r="L4" s="15" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="18" t="s">
-        <v>41</v>
+      <c r="D5" s="14" t="s">
+        <v>40</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="15" t="s">
+      <c r="G5" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="H5" s="18" t="s">
-        <v>41</v>
+      <c r="H5" s="14" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="18" t="s">
-        <v>42</v>
+      <c r="D6" s="14" t="s">
+        <v>41</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="15" t="s">
+      <c r="G6" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="H6" s="18" t="s">
-        <v>41</v>
+      <c r="H6" s="14" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="18" t="s">
-        <v>42</v>
+      <c r="D7" s="14" t="s">
+        <v>41</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G7" s="15" t="s">
+      <c r="G7" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="H7" s="18" t="s">
-        <v>42</v>
+      <c r="H7" s="14" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="18" t="s">
-        <v>41</v>
+      <c r="D8" s="14" t="s">
+        <v>40</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G8" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="H8" s="18" t="s">
-        <v>41</v>
+      <c r="G8" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="H8" s="14" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="C9" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="18" t="s">
-        <v>42</v>
+      <c r="D9" s="14" t="s">
+        <v>41</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G9" s="15" t="s">
+      <c r="G9" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="H9" s="18" t="s">
-        <v>41</v>
+      <c r="H9" s="14" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
       <c r="F10" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="G10" s="15" t="s">
+      <c r="G10" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="H10" s="18" t="s">
-        <v>42</v>
+      <c r="H10" s="14" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
       <c r="F11" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G11" s="15" t="s">
+      <c r="G11" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="H11" s="18" t="s">
-        <v>42</v>
+      <c r="H11" s="14" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.25">
       <c r="F12" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G12" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="H12" s="18" t="s">
-        <v>41</v>
+      <c r="G12" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="H12" s="14" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.25">
       <c r="F13" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="G13" s="15" t="s">
+      <c r="G13" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="H13" s="18" t="s">
-        <v>41</v>
+      <c r="H13" s="14" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.25">
       <c r="F14" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G14" s="15" t="s">
+      <c r="G14" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="H14" s="18" t="s">
-        <v>41</v>
+      <c r="H14" s="14" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F15" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G15" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="H15" s="18" t="s">
-        <v>42</v>
+      <c r="G15" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="H15" s="14" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -4800,7 +4800,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:P18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
@@ -4821,101 +4821,101 @@
   <sheetData>
     <row r="1" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:16" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="34"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="42"/>
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="36" t="s">
-        <v>40</v>
-      </c>
-      <c r="D3" s="36" t="s">
-        <v>35</v>
-      </c>
-      <c r="E3" s="37" t="s">
+      <c r="C3" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="37" t="s">
+      <c r="F3" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="37" t="s">
+      <c r="G3" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="13" t="s">
+      <c r="H3" s="9" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B4" s="42">
+      <c r="B4" s="33">
         <v>1</v>
       </c>
-      <c r="C4" s="42">
+      <c r="C4" s="33">
         <v>2</v>
       </c>
-      <c r="D4" s="28" t="s">
+      <c r="D4" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="E4" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="E4" s="27" t="s">
+      <c r="F4" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>46</v>
       </c>
       <c r="H4" s="4">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B5" s="20">
+      <c r="B5" s="16">
         <v>2</v>
       </c>
-      <c r="C5" s="42">
+      <c r="C5" s="33">
         <v>1</v>
       </c>
-      <c r="D5" s="28" t="s">
-        <v>43</v>
-      </c>
-      <c r="E5" s="28" t="s">
-        <v>43</v>
+      <c r="D5" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" s="22" t="s">
+        <v>42</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H5" s="4">
         <v>0.5</v>
       </c>
     </row>
     <row r="6" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="21">
+      <c r="B6" s="17">
         <v>3</v>
       </c>
-      <c r="C6" s="42">
+      <c r="C6" s="33">
         <v>1</v>
       </c>
-      <c r="D6" s="28" t="s">
-        <v>43</v>
-      </c>
-      <c r="E6" s="28" t="s">
-        <v>43</v>
-      </c>
-      <c r="F6" s="25" t="s">
+      <c r="D6" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="G6" s="19" t="s">
         <v>45</v>
-      </c>
-      <c r="G6" s="25" t="s">
-        <v>46</v>
       </c>
       <c r="H6" s="6">
         <v>5</v>
@@ -4923,219 +4923,219 @@
     </row>
     <row r="7" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="2:16" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="32" t="s">
+      <c r="B8" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="33"/>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="33"/>
-      <c r="G8" s="33"/>
-      <c r="H8" s="33"/>
-      <c r="I8" s="33"/>
-      <c r="J8" s="33"/>
-      <c r="K8" s="33"/>
-      <c r="L8" s="33"/>
-      <c r="M8" s="33"/>
-      <c r="N8" s="34"/>
+      <c r="C8" s="41"/>
+      <c r="D8" s="41"/>
+      <c r="E8" s="41"/>
+      <c r="F8" s="41"/>
+      <c r="G8" s="41"/>
+      <c r="H8" s="41"/>
+      <c r="I8" s="41"/>
+      <c r="J8" s="41"/>
+      <c r="K8" s="41"/>
+      <c r="L8" s="41"/>
+      <c r="M8" s="41"/>
+      <c r="N8" s="42"/>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B9" s="35" t="s">
+      <c r="B9" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="37" t="s">
-        <v>39</v>
-      </c>
-      <c r="D9" s="37" t="s">
+      <c r="C9" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="37" t="s">
+      <c r="E9" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="F9" s="38" t="s">
+      <c r="F9" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="G9" s="31" t="s">
+      <c r="G9" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="H9" s="38" t="s">
+      <c r="H9" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="I9" s="38" t="s">
+      <c r="I9" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="J9" s="38" t="s">
+      <c r="J9" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="K9" s="38" t="s">
+      <c r="K9" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="L9" s="38" t="s">
+      <c r="L9" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="M9" s="38" t="s">
+      <c r="M9" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="N9" s="39" t="s">
+      <c r="N9" s="30" t="s">
         <v>20</v>
       </c>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B10" s="20">
+      <c r="B10" s="16">
         <v>1</v>
       </c>
-      <c r="C10" s="43">
+      <c r="C10" s="34">
         <v>2</v>
       </c>
       <c r="D10" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="F10" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="F10" s="43" t="s">
-        <v>54</v>
-      </c>
       <c r="G10" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="H10" s="34">
+        <v>25</v>
+      </c>
+      <c r="I10" s="34"/>
+      <c r="J10" s="34"/>
+      <c r="K10" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="H10" s="43">
-        <v>25</v>
-      </c>
-      <c r="I10" s="43"/>
-      <c r="J10" s="43"/>
-      <c r="K10" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="L10" s="43">
+      <c r="L10" s="34">
         <v>2552</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="N10" s="29" t="s">
-        <v>63</v>
+        <v>67</v>
+      </c>
+      <c r="N10" s="23" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B11" s="20">
+      <c r="B11" s="16">
         <v>2</v>
       </c>
-      <c r="C11" s="43">
+      <c r="C11" s="34">
         <v>2</v>
       </c>
       <c r="D11" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="E11" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="F11" s="43" t="s">
-        <v>55</v>
+      <c r="F11" s="34" t="s">
+        <v>54</v>
       </c>
       <c r="G11" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="H11" s="34">
+        <v>23</v>
+      </c>
+      <c r="I11" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="H11" s="43">
-        <v>23</v>
-      </c>
-      <c r="I11" s="43" t="s">
+      <c r="J11" s="34">
+        <v>2</v>
+      </c>
+      <c r="K11" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="J11" s="43">
-        <v>2</v>
-      </c>
-      <c r="K11" s="2" t="s">
+      <c r="L11" s="34">
+        <v>1100</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="N11" s="23" t="s">
         <v>61</v>
-      </c>
-      <c r="L11" s="43">
-        <v>1100</v>
-      </c>
-      <c r="M11" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="N11" s="29" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="12" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="21">
+      <c r="B12" s="17">
         <v>3</v>
       </c>
-      <c r="C12" s="44">
+      <c r="C12" s="35">
         <v>1</v>
       </c>
-      <c r="D12" s="25" t="s">
+      <c r="D12" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="E12" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="E12" s="25" t="s">
-        <v>49</v>
-      </c>
-      <c r="F12" s="44" t="s">
-        <v>56</v>
-      </c>
-      <c r="G12" s="25" t="s">
+      <c r="F12" s="35" t="s">
+        <v>55</v>
+      </c>
+      <c r="G12" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="H12" s="35">
+        <v>14</v>
+      </c>
+      <c r="I12" s="35"/>
+      <c r="J12" s="35">
+        <v>1</v>
+      </c>
+      <c r="K12" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="H12" s="44">
-        <v>14</v>
-      </c>
-      <c r="I12" s="44"/>
-      <c r="J12" s="44">
-        <v>1</v>
-      </c>
-      <c r="K12" s="25" t="s">
+      <c r="L12" s="35">
+        <v>7000</v>
+      </c>
+      <c r="M12" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="L12" s="44">
-        <v>7000</v>
-      </c>
-      <c r="M12" s="25" t="s">
-        <v>67</v>
-      </c>
-      <c r="N12" s="30" t="s">
-        <v>64</v>
+      <c r="N12" s="24" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="13" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="2:16" s="22" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B14" s="23" t="s">
+    <row r="14" spans="2:16" s="18" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B14" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="24"/>
+      <c r="C14" s="44"/>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B15" s="40" t="s">
+      <c r="B15" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="41" t="s">
+      <c r="C15" s="32" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B16" s="20">
+      <c r="B16" s="16">
         <v>1</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" s="20">
+      <c r="B17" s="16">
         <v>2</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="21">
+      <c r="B18" s="17">
         <v>3</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#3 Define Database for TimeRecorder
Insert to the testdata the "DefaultPasswort" value. (tblLogin => table)
</commit_message>
<xml_diff>
--- a/TimeRecorder_Desktop/Planing/TimeRecorderDatabasePlaning.xlsx
+++ b/TimeRecorder_Desktop/Planing/TimeRecorderDatabasePlaning.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="663" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ERM" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="81">
   <si>
     <t>tblTime</t>
   </si>
@@ -259,13 +259,16 @@
     <t>764d333399f0fe417fd8fec51a2e17f42a7a2076</t>
   </si>
   <si>
-    <t>SHA1 = 160-bit hash value</t>
-  </si>
-  <si>
-    <t>NVARCHAR(20)</t>
-  </si>
-  <si>
-    <t>160 bit = 20 Byte</t>
+    <t>DefaultPassword</t>
+  </si>
+  <si>
+    <t>BIT</t>
+  </si>
+  <si>
+    <t>SHA-1 generates a 160-bit hash value. You can use CHAR(40) or BINARY(20)</t>
+  </si>
+  <si>
+    <t>NVARCHAR(40)</t>
   </si>
 </sst>
 </file>
@@ -326,10 +329,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="11.25"/>
       <color rgb="FF242729"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -340,7 +344,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -620,12 +624,36 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -718,11 +746,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -739,7 +773,18 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -5338,7 +5383,7 @@
   <dimension ref="B1:L15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5349,8 +5394,8 @@
     <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5493,7 +5538,7 @@
       </c>
       <c r="K7" s="41"/>
     </row>
-    <row r="8" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>2</v>
       </c>
@@ -5541,17 +5586,17 @@
       <c r="H9" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="J9" s="5" t="s">
+      <c r="J9" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="K9" s="13" t="s">
-        <v>78</v>
+      <c r="K9" s="11" t="s">
+        <v>80</v>
       </c>
       <c r="L9" s="15" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F10" s="3" t="s">
         <v>16</v>
       </c>
@@ -5561,8 +5606,14 @@
       <c r="H10" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="K10" s="47" t="s">
+      <c r="J10" s="5" t="s">
         <v>77</v>
+      </c>
+      <c r="K10" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="L10" s="15" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
@@ -5575,7 +5626,7 @@
       <c r="H11" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="K11" t="s">
+      <c r="K11" s="42" t="s">
         <v>79</v>
       </c>
     </row>
@@ -5589,6 +5640,7 @@
       <c r="H12" s="14" t="s">
         <v>40</v>
       </c>
+      <c r="K12" s="43"/>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.25">
       <c r="F13" s="3" t="s">
@@ -5600,6 +5652,7 @@
       <c r="H13" s="14" t="s">
         <v>40</v>
       </c>
+      <c r="K13" s="43"/>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.25">
       <c r="F14" s="3" t="s">
@@ -5624,11 +5677,12 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="J7:K7"/>
+    <mergeCell ref="K11:K13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5639,8 +5693,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:P18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5649,7 +5703,7 @@
     <col min="3" max="3" width="20.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="21.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="43" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="5.28515625" bestFit="1" customWidth="1"/>
@@ -5661,15 +5715,15 @@
   <sheetData>
     <row r="1" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:16" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="44"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="46"/>
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B3" s="26" t="s">
@@ -5763,21 +5817,21 @@
     </row>
     <row r="7" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="2:16" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="42" t="s">
+      <c r="B8" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="43"/>
-      <c r="D8" s="43"/>
-      <c r="E8" s="43"/>
-      <c r="F8" s="43"/>
-      <c r="G8" s="43"/>
-      <c r="H8" s="43"/>
-      <c r="I8" s="43"/>
-      <c r="J8" s="43"/>
-      <c r="K8" s="43"/>
-      <c r="L8" s="43"/>
-      <c r="M8" s="43"/>
-      <c r="N8" s="44"/>
+      <c r="C8" s="45"/>
+      <c r="D8" s="45"/>
+      <c r="E8" s="45"/>
+      <c r="F8" s="45"/>
+      <c r="G8" s="45"/>
+      <c r="H8" s="45"/>
+      <c r="I8" s="45"/>
+      <c r="J8" s="45"/>
+      <c r="K8" s="45"/>
+      <c r="L8" s="45"/>
+      <c r="M8" s="45"/>
+      <c r="N8" s="46"/>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B9" s="26" t="s">
@@ -5941,14 +5995,15 @@
     </row>
     <row r="13" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="2:16" s="18" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="42" t="s">
+      <c r="B14" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="44"/>
-      <c r="E14" s="45" t="s">
+      <c r="C14" s="46"/>
+      <c r="E14" s="47" t="s">
         <v>70</v>
       </c>
-      <c r="F14" s="46"/>
+      <c r="F14" s="52"/>
+      <c r="G14" s="48"/>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B15" s="34" t="s">
@@ -5960,8 +6015,11 @@
       <c r="E15" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="F15" s="35" t="s">
+      <c r="F15" s="51" t="s">
         <v>73</v>
+      </c>
+      <c r="G15" s="35" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.25">
@@ -5974,11 +6032,14 @@
       <c r="E16" s="16">
         <v>2</v>
       </c>
-      <c r="F16" s="4" t="s">
+      <c r="F16" s="2" t="s">
         <v>74</v>
       </c>
+      <c r="G16" s="49">
+        <v>0</v>
+      </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="16">
         <v>2</v>
       </c>
@@ -5988,11 +6049,14 @@
       <c r="E17" s="16">
         <v>1</v>
       </c>
-      <c r="F17" s="4" t="s">
+      <c r="F17" s="2" t="s">
         <v>75</v>
       </c>
+      <c r="G17" s="49">
+        <v>0</v>
+      </c>
     </row>
-    <row r="18" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="17">
         <v>3</v>
       </c>
@@ -6002,8 +6066,11 @@
       <c r="E18" s="17">
         <v>3</v>
       </c>
-      <c r="F18" s="6" t="s">
+      <c r="F18" s="19" t="s">
         <v>76</v>
+      </c>
+      <c r="G18" s="50">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -6011,7 +6078,7 @@
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="B8:N8"/>
     <mergeCell ref="B14:C14"/>
-    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E14:G14"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="N11" r:id="rId1"/>

</xml_diff>